<commit_message>
ngày cuối rồi. 6h toist thuyết trình mà giờ 2h giờ sáng làm mất file ui
</commit_message>
<xml_diff>
--- a/Data/Export/6A1_Student_List.xlsx
+++ b/Data/Export/6A1_Student_List.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,185 +424,136 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>Họ tên</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>Điểm miệng cột 1</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>gender</t>
+          <t>Điểm miệng cột 2</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>dob</t>
+          <t>Điểm 15p cột 1</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>parent_account</t>
+          <t>Điểm 15p cột 2</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>parent_password</t>
+          <t>Điểm 1 tiết cột 1</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>class</t>
+          <t>Điểm 1 tiết cột 2</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Điểm Giữa kỳ</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Điểm Cuối kỳ</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>MS90027</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Lý Sujoi</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Nam</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>2025-06-20</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>phhs_MS90027</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>phhs_MS90027_1234</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>6A1</t>
-        </is>
+          <t>Lý Anh Hiển</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>MS01118</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Nguyễn Văn B</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Nữ</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>2012-02-02</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>phhs_MS01118</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>phhs_MS01118_1234</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>6A1</t>
-        </is>
+          <t>Nguyễn Dương Thanh Trúc</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E3" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3" t="n">
+        <v>2</v>
+      </c>
+      <c r="G3" t="n">
+        <v>2</v>
+      </c>
+      <c r="H3" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>MS83708</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Nguyễn Văn D</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Nữ</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>2012-04-04</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>phhs_MS83708</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>phhs_MS83708_1234</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>6A1</t>
-        </is>
+          <t>Nguyễn Văn G</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>MS25039</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Lý ANh Hiển</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Nam</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>2012-05-05</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>phhs_MS25039</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>phhs_MS25039_1234</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>6A1</t>
+          <t>Lý Suni</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>3</v>
+      </c>
+      <c r="D5" t="n">
+        <v>4</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Lý Money</t>
         </is>
       </c>
     </row>

</xml_diff>